<commit_message>
Published state of ETDataset on 14 August 2015
</commit_message>
<xml_diff>
--- a/carriers_source_analyses/biodiesel.carrier.xlsx
+++ b/carriers_source_analyses/biodiesel.carrier.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="16140" tabRatio="762" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="762" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -17,6 +17,7 @@
   <externalReferences>
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="exchange_rate_2011_2010">#REF!</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="181">
   <si>
     <t>Source</t>
   </si>
@@ -508,12 +509,6 @@
     <t>Average</t>
   </si>
   <si>
-    <t>UFOP website</t>
-  </si>
-  <si>
-    <t>UFOP</t>
-  </si>
-  <si>
     <t>Price (EUR/100l)</t>
   </si>
   <si>
@@ -521,13 +516,106 @@
   </si>
   <si>
     <t>EUR/L</t>
+  </si>
+  <si>
+    <t>European Commission - Weekly Oil Bulletin</t>
+  </si>
+  <si>
+    <t>http://ec.europa.eu/energy/observatory/oil/bulletin_en.htm</t>
+  </si>
+  <si>
+    <t>Calculate monthly average</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>ExchangeRateTo €</t>
+  </si>
+  <si>
+    <t>No taxes</t>
+  </si>
+  <si>
+    <t>1000L</t>
+  </si>
+  <si>
+    <t>EUR/1000L</t>
+  </si>
+  <si>
+    <t>Incl taxes</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>VAT</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Excise</t>
+  </si>
+  <si>
+    <t>Other indirect</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>EUR/L (inc tax)</t>
+  </si>
+  <si>
+    <t>diesel</t>
+  </si>
+  <si>
+    <t>Gas oil automobileAutomotive gas oilDieselkraftstoff(I)</t>
+  </si>
+  <si>
+    <t>Excise rate</t>
+  </si>
+  <si>
+    <t>Oher indirect tax</t>
+  </si>
+  <si>
+    <t>VAT rate</t>
+  </si>
+  <si>
+    <t>http://www.biotanken.nl/brandstoffen/biodiesel.html</t>
+  </si>
+  <si>
+    <t>price difference per liter biodiesel with normal diesel</t>
+  </si>
+  <si>
+    <t>normal diesel, pump prices (incl tax)</t>
+  </si>
+  <si>
+    <t>Biodiesel estimated pump price (incl tax)</t>
+  </si>
+  <si>
+    <t>Biodiesel estimated pump price (Excl tax)</t>
+  </si>
+  <si>
+    <t>EC_Oil Bulletin</t>
+  </si>
+  <si>
+    <t>biotanken.nl</t>
+  </si>
+  <si>
+    <t>EC Oil bulletin</t>
+  </si>
+  <si>
+    <t>Assumed dependent on nromal diesel price</t>
+  </si>
+  <si>
+    <t>EC Oil Bulletin and biotanken.nl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="7">
+  <numFmts count="10">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
@@ -535,13 +623,23 @@
     <numFmt numFmtId="168" formatCode="0.000000000"/>
     <numFmt numFmtId="169" formatCode="0.0000000000"/>
     <numFmt numFmtId="170" formatCode="0.00000000000"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="172" formatCode="0.00000"/>
+    <numFmt numFmtId="173" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="47" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -771,8 +869,65 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Lettertype hoofdtekst"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF900000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF900000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="16"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="16"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -851,8 +1006,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFF58C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF666699"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1171,652 +1362,804 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="332">
+  <cellStyleXfs count="335">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="183" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="26" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="183" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="25" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="183" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="26" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="12" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="183" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="183" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="38" fillId="15" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="16" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="40" fillId="16" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="41" fillId="17" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="16" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="17" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="24" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="14" fontId="44" fillId="16" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="25" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="45" fillId="16" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="46" fillId="19" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="24" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="172" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="44" fillId="18" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="332">
+  <cellStyles count="335">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2059,6 +2402,9 @@
     <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2828,6 +3174,158 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>472</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>476</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9334500" y="104609900"/>
+          <a:ext cx="7137400" cy="1562100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>480</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>487</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9296400" y="106337100"/>
+          <a:ext cx="7391400" cy="1498600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>488</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>497</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9296400" y="107962700"/>
+          <a:ext cx="7213600" cy="1816100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>512</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>566</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9296400" y="103365300"/>
+          <a:ext cx="6350000" cy="10312400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2945,6 +3443,26 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover sheet"/>
+      <sheetName val="Dashboard"/>
+      <sheetName val="carrier_manager.xlsm"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="update_attributes"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3494,7 +4012,9 @@
   </sheetPr>
   <dimension ref="B1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3518,28 +4038,28 @@
       <c r="G1" s="36"/>
     </row>
     <row r="2" spans="2:11" ht="15" customHeight="1">
-      <c r="B2" s="175" t="s">
+      <c r="B2" s="174" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="177"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="176"/>
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="178"/>
-      <c r="C3" s="179"/>
-      <c r="D3" s="179"/>
-      <c r="E3" s="180"/>
+      <c r="B3" s="177"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="179"/>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="181"/>
-      <c r="C4" s="182"/>
-      <c r="D4" s="182"/>
-      <c r="E4" s="183"/>
+      <c r="B4" s="180"/>
+      <c r="C4" s="181"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="182"/>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
     </row>
@@ -3634,13 +4154,13 @@
       </c>
       <c r="E11" s="173">
         <f>'Research data'!G7</f>
-        <v>2.2042255648181703E-2</v>
+        <v>2.9081568260948144E-2</v>
       </c>
       <c r="F11" s="37"/>
       <c r="G11" s="131"/>
       <c r="H11" s="32"/>
-      <c r="I11" s="174" t="s">
-        <v>148</v>
+      <c r="I11" s="212" t="s">
+        <v>180</v>
       </c>
       <c r="J11" s="46"/>
     </row>
@@ -3732,7 +4252,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="2049" r:id="rId3" name="export_data">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!update_attributes">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[3]!update_attributes">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>6</xdr:col>
@@ -3795,30 +4315,30 @@
       <c r="G1" s="36"/>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1">
-      <c r="B2" s="175" t="s">
+      <c r="B2" s="174" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="177"/>
+      <c r="C2" s="175"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="176"/>
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="178"/>
-      <c r="C3" s="179"/>
-      <c r="D3" s="179"/>
-      <c r="E3" s="180"/>
+      <c r="B3" s="177"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="178"/>
+      <c r="E3" s="179"/>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="184" t="s">
+      <c r="B4" s="183" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="185"/>
-      <c r="D4" s="185"/>
-      <c r="E4" s="186"/>
+      <c r="C4" s="184"/>
+      <c r="D4" s="184"/>
+      <c r="E4" s="185"/>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
     </row>
@@ -4259,7 +4779,7 @@
   <dimension ref="B1:Q36"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4330,7 +4850,7 @@
       </c>
       <c r="N3" s="69"/>
       <c r="O3" s="69" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="P3" s="69"/>
       <c r="Q3" s="1" t="s">
@@ -4418,7 +4938,7 @@
       </c>
       <c r="G7" s="172">
         <f>O7</f>
-        <v>2.2042255648181703E-2</v>
+        <v>2.9081568260948144E-2</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="18"/>
@@ -4428,11 +4948,13 @@
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
       <c r="O7" s="171">
-        <f>Notes!H454</f>
-        <v>2.2042255648181703E-2</v>
+        <f>Notes!F528</f>
+        <v>2.9081568260948144E-2</v>
       </c>
       <c r="P7" s="16"/>
-      <c r="Q7" s="145"/>
+      <c r="Q7" s="211" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="8" spans="2:17" s="6" customFormat="1" ht="16" thickBot="1">
       <c r="B8" s="5"/>
@@ -5081,7 +5603,7 @@
   <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5371,7 +5893,7 @@
       </c>
       <c r="D18" s="62"/>
       <c r="E18" s="148" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="F18" s="148"/>
       <c r="G18" s="62"/>
@@ -5379,12 +5901,19 @@
       <c r="I18" s="70"/>
       <c r="J18" s="62"/>
       <c r="K18" s="68"/>
-      <c r="L18" s="66"/>
-    </row>
-    <row r="19" spans="2:12">
+      <c r="L18" s="66" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="16">
       <c r="B19" s="54"/>
-      <c r="E19" s="149"/>
+      <c r="E19" s="149" t="s">
+        <v>176</v>
+      </c>
       <c r="F19" s="149"/>
+      <c r="L19" s="190" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="20" spans="2:12">
       <c r="B20" s="54"/>
@@ -5404,6 +5933,9 @@
       <c r="F22" s="149"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L19" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -5416,10 +5948,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y454"/>
+  <dimension ref="A1:Y530"/>
   <sheetViews>
-    <sheetView topLeftCell="A418" workbookViewId="0">
-      <selection activeCell="I446" sqref="I446"/>
+    <sheetView topLeftCell="A484" workbookViewId="0">
+      <selection activeCell="C470" sqref="C470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11292,7 +11824,7 @@
     </row>
     <row r="447" spans="2:25">
       <c r="F447" s="169" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G447" s="169" t="s">
         <v>140</v>
@@ -11378,7 +11910,7 @@
         <v>72.977499999999992</v>
       </c>
       <c r="I452" s="169" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="453" spans="5:9">
@@ -11387,7 +11919,7 @@
         <v>0.72977499999999995</v>
       </c>
       <c r="I453" s="169" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="454" spans="5:9">
@@ -11399,13 +11931,1513 @@
         <v>62</v>
       </c>
     </row>
+    <row r="466" spans="1:25" ht="16" thickBot="1"/>
+    <row r="467" spans="1:25" s="187" customFormat="1">
+      <c r="A467" s="159"/>
+      <c r="B467" s="186"/>
+      <c r="C467" s="186" t="s">
+        <v>25</v>
+      </c>
+      <c r="D467" s="186" t="s">
+        <v>65</v>
+      </c>
+      <c r="E467" s="186"/>
+      <c r="F467" s="186" t="s">
+        <v>32</v>
+      </c>
+      <c r="G467" s="186"/>
+      <c r="H467" s="186"/>
+      <c r="I467" s="186"/>
+      <c r="J467" s="186"/>
+      <c r="K467" s="186"/>
+      <c r="L467" s="186"/>
+      <c r="M467" s="186"/>
+      <c r="N467" s="186"/>
+      <c r="O467" s="186"/>
+      <c r="P467" s="186"/>
+      <c r="Q467" s="186"/>
+      <c r="R467" s="186"/>
+      <c r="S467" s="186"/>
+      <c r="T467" s="186"/>
+      <c r="U467" s="186"/>
+      <c r="V467" s="159"/>
+      <c r="W467" s="159"/>
+      <c r="X467" s="159"/>
+      <c r="Y467" s="159"/>
+    </row>
+    <row r="468" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A468" s="188"/>
+      <c r="B468" s="189"/>
+      <c r="C468" s="139"/>
+      <c r="D468" s="139"/>
+      <c r="E468" s="139"/>
+      <c r="F468" s="139"/>
+      <c r="G468" s="139"/>
+      <c r="H468" s="139"/>
+      <c r="I468" s="139"/>
+      <c r="J468" s="139"/>
+      <c r="K468" s="139"/>
+      <c r="L468" s="139"/>
+      <c r="M468" s="139"/>
+      <c r="N468" s="139"/>
+      <c r="O468" s="139"/>
+      <c r="P468" s="139"/>
+      <c r="Q468" s="139"/>
+      <c r="R468" s="139"/>
+      <c r="S468" s="139"/>
+      <c r="T468" s="139"/>
+      <c r="U468" s="139"/>
+      <c r="V468" s="139"/>
+      <c r="W468" s="139"/>
+      <c r="X468" s="139"/>
+      <c r="Y468" s="139"/>
+    </row>
+    <row r="469" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A469" s="188"/>
+      <c r="B469" s="189"/>
+      <c r="C469" s="159" t="s">
+        <v>150</v>
+      </c>
+      <c r="D469" s="139"/>
+      <c r="E469" s="139"/>
+      <c r="F469" s="139"/>
+      <c r="G469" s="139"/>
+      <c r="H469" s="139"/>
+      <c r="I469" s="139"/>
+      <c r="J469" s="139"/>
+      <c r="K469" s="139"/>
+      <c r="L469" s="139"/>
+      <c r="M469" s="139"/>
+      <c r="N469" s="139"/>
+      <c r="O469" s="139"/>
+      <c r="P469" s="139"/>
+      <c r="Q469" s="139"/>
+      <c r="R469" s="139"/>
+      <c r="S469" s="139"/>
+      <c r="T469" s="139"/>
+      <c r="U469" s="139"/>
+      <c r="V469" s="139"/>
+      <c r="W469" s="139"/>
+      <c r="X469" s="139"/>
+      <c r="Y469" s="139"/>
+    </row>
+    <row r="470" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A470" s="188"/>
+      <c r="B470" s="189"/>
+      <c r="C470" s="190" t="s">
+        <v>151</v>
+      </c>
+      <c r="D470" s="139"/>
+      <c r="E470" s="139"/>
+      <c r="F470" s="139"/>
+      <c r="G470" s="139"/>
+      <c r="H470" s="139"/>
+      <c r="I470" s="139"/>
+      <c r="J470" s="139"/>
+      <c r="K470" s="139"/>
+      <c r="L470" s="139"/>
+      <c r="M470" s="139"/>
+      <c r="N470" s="139"/>
+      <c r="O470" s="139"/>
+      <c r="P470" s="139"/>
+      <c r="Q470" s="139"/>
+      <c r="R470" s="139"/>
+      <c r="S470" s="139"/>
+      <c r="T470" s="139"/>
+      <c r="U470" s="139"/>
+      <c r="V470" s="139"/>
+      <c r="W470" s="139"/>
+      <c r="X470" s="139"/>
+      <c r="Y470" s="139"/>
+    </row>
+    <row r="471" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A471" s="188"/>
+      <c r="B471" s="189"/>
+      <c r="C471" s="139"/>
+      <c r="D471" s="188"/>
+      <c r="E471" s="139"/>
+      <c r="F471" s="139"/>
+      <c r="G471" s="139"/>
+      <c r="H471" s="139"/>
+      <c r="I471" s="139"/>
+      <c r="J471" s="139"/>
+      <c r="K471" s="139"/>
+      <c r="L471" s="139"/>
+      <c r="M471" s="139"/>
+      <c r="N471" s="139"/>
+      <c r="O471" s="139"/>
+      <c r="P471" s="139"/>
+      <c r="Q471" s="139"/>
+      <c r="R471" s="139"/>
+      <c r="S471" s="139"/>
+      <c r="T471" s="139"/>
+      <c r="U471" s="139"/>
+      <c r="V471" s="139"/>
+      <c r="W471" s="139"/>
+      <c r="X471" s="139"/>
+      <c r="Y471" s="139"/>
+    </row>
+    <row r="472" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A472" s="188"/>
+      <c r="B472" s="189"/>
+      <c r="C472" s="139"/>
+      <c r="D472" s="139" t="s">
+        <v>152</v>
+      </c>
+      <c r="E472" s="139"/>
+      <c r="F472" s="139"/>
+      <c r="G472" s="139"/>
+      <c r="H472" s="139"/>
+      <c r="I472" s="139"/>
+      <c r="J472" s="139"/>
+      <c r="K472" s="139"/>
+      <c r="L472" s="139"/>
+      <c r="M472" s="139"/>
+      <c r="N472" s="139"/>
+      <c r="O472" s="139"/>
+      <c r="P472" s="139"/>
+      <c r="Q472" s="139"/>
+      <c r="R472" s="139"/>
+      <c r="S472" s="139"/>
+      <c r="T472" s="139"/>
+      <c r="U472" s="139"/>
+      <c r="V472" s="139"/>
+      <c r="W472" s="139"/>
+      <c r="X472" s="139"/>
+      <c r="Y472" s="139"/>
+    </row>
+    <row r="473" spans="1:25" s="187" customFormat="1" ht="50">
+      <c r="A473" s="188"/>
+      <c r="B473" s="189"/>
+      <c r="C473" s="139"/>
+      <c r="D473" s="191" t="s">
+        <v>3</v>
+      </c>
+      <c r="E473" s="188"/>
+      <c r="F473" s="139"/>
+      <c r="G473" s="139"/>
+      <c r="H473" s="192" t="s">
+        <v>153</v>
+      </c>
+      <c r="I473" s="193" t="s">
+        <v>154</v>
+      </c>
+      <c r="J473" s="194" t="s">
+        <v>167</v>
+      </c>
+      <c r="K473" s="195" t="s">
+        <v>167</v>
+      </c>
+      <c r="L473" s="139"/>
+      <c r="M473" s="139"/>
+      <c r="N473" s="139"/>
+      <c r="O473" s="139"/>
+      <c r="P473" s="139"/>
+      <c r="Q473" s="139"/>
+      <c r="R473" s="139"/>
+      <c r="S473" s="139"/>
+      <c r="T473" s="139"/>
+      <c r="U473" s="139"/>
+      <c r="V473" s="139"/>
+    </row>
+    <row r="474" spans="1:25" s="187" customFormat="1" ht="17" thickBot="1">
+      <c r="A474" s="188"/>
+      <c r="B474" s="189"/>
+      <c r="C474" s="139"/>
+      <c r="D474" s="139" t="s">
+        <v>155</v>
+      </c>
+      <c r="E474" s="188"/>
+      <c r="F474" s="139"/>
+      <c r="G474" s="139"/>
+      <c r="H474" s="196"/>
+      <c r="I474" s="197"/>
+      <c r="J474" s="198" t="s">
+        <v>156</v>
+      </c>
+      <c r="K474" s="199" t="s">
+        <v>156</v>
+      </c>
+      <c r="L474" s="139"/>
+      <c r="M474" s="139"/>
+      <c r="N474" s="139"/>
+      <c r="O474" s="139"/>
+      <c r="P474" s="139"/>
+      <c r="Q474" s="139"/>
+      <c r="R474" s="139"/>
+      <c r="S474" s="139"/>
+      <c r="T474" s="139"/>
+      <c r="U474" s="139"/>
+      <c r="V474" s="139"/>
+    </row>
+    <row r="475" spans="1:25" s="187" customFormat="1" ht="17" thickBot="1">
+      <c r="A475" s="188"/>
+      <c r="B475" s="189"/>
+      <c r="C475" s="139"/>
+      <c r="D475" s="139"/>
+      <c r="E475" s="188" t="s">
+        <v>166</v>
+      </c>
+      <c r="F475" s="200">
+        <f>AVERAGE(J475:J479)</f>
+        <v>549.61</v>
+      </c>
+      <c r="G475" s="139" t="s">
+        <v>157</v>
+      </c>
+      <c r="H475" s="201">
+        <v>42219</v>
+      </c>
+      <c r="I475" s="202">
+        <v>1</v>
+      </c>
+      <c r="J475" s="206">
+        <v>518.20000000000005</v>
+      </c>
+      <c r="K475" s="203">
+        <v>1220</v>
+      </c>
+      <c r="L475" s="139"/>
+      <c r="M475" s="139"/>
+      <c r="N475" s="139"/>
+      <c r="O475" s="139"/>
+      <c r="P475" s="139"/>
+      <c r="Q475" s="139"/>
+      <c r="R475" s="139"/>
+      <c r="S475" s="139"/>
+      <c r="T475" s="139"/>
+      <c r="U475" s="139"/>
+      <c r="V475" s="139"/>
+    </row>
+    <row r="476" spans="1:25" s="187" customFormat="1" ht="17" thickBot="1">
+      <c r="A476" s="188"/>
+      <c r="B476" s="189"/>
+      <c r="C476" s="139"/>
+      <c r="D476" s="139"/>
+      <c r="E476" s="188" t="s">
+        <v>166</v>
+      </c>
+      <c r="F476" s="204">
+        <f>F475/1000</f>
+        <v>0.54961000000000004</v>
+      </c>
+      <c r="G476" s="139" t="s">
+        <v>149</v>
+      </c>
+      <c r="H476" s="201">
+        <v>42212</v>
+      </c>
+      <c r="I476" s="202">
+        <v>1</v>
+      </c>
+      <c r="J476" s="206">
+        <v>533.91</v>
+      </c>
+      <c r="K476" s="203">
+        <v>1239</v>
+      </c>
+      <c r="L476" s="139"/>
+      <c r="M476" s="139"/>
+      <c r="N476" s="139"/>
+      <c r="O476" s="139"/>
+      <c r="P476" s="139"/>
+      <c r="Q476" s="139"/>
+      <c r="R476" s="139"/>
+      <c r="S476" s="139"/>
+      <c r="T476" s="139"/>
+      <c r="U476" s="139"/>
+      <c r="V476" s="139"/>
+    </row>
+    <row r="477" spans="1:25" s="187" customFormat="1" ht="17" thickBot="1">
+      <c r="A477" s="188"/>
+      <c r="B477" s="189"/>
+      <c r="C477" s="139"/>
+      <c r="D477" s="139"/>
+      <c r="E477" s="139"/>
+      <c r="F477" s="139"/>
+      <c r="G477" s="139"/>
+      <c r="H477" s="201">
+        <v>42205</v>
+      </c>
+      <c r="I477" s="202">
+        <v>1</v>
+      </c>
+      <c r="J477" s="206">
+        <v>547.13</v>
+      </c>
+      <c r="K477" s="203">
+        <v>1255</v>
+      </c>
+      <c r="L477" s="139"/>
+      <c r="M477" s="139"/>
+      <c r="N477" s="139"/>
+      <c r="O477" s="139"/>
+      <c r="P477" s="139"/>
+      <c r="Q477" s="139"/>
+      <c r="R477" s="139"/>
+      <c r="S477" s="139"/>
+      <c r="T477" s="139"/>
+      <c r="U477" s="139"/>
+      <c r="V477" s="139"/>
+    </row>
+    <row r="478" spans="1:25" s="187" customFormat="1" ht="17" thickBot="1">
+      <c r="A478" s="188"/>
+      <c r="B478" s="189"/>
+      <c r="C478" s="139"/>
+      <c r="D478" s="139" t="s">
+        <v>158</v>
+      </c>
+      <c r="E478" s="188" t="s">
+        <v>166</v>
+      </c>
+      <c r="F478" s="200">
+        <f>AVERAGE(K475:K479)</f>
+        <v>1258</v>
+      </c>
+      <c r="G478" s="139" t="s">
+        <v>157</v>
+      </c>
+      <c r="H478" s="201">
+        <v>42198</v>
+      </c>
+      <c r="I478" s="202">
+        <v>1</v>
+      </c>
+      <c r="J478" s="206">
+        <v>568.62</v>
+      </c>
+      <c r="K478" s="203">
+        <v>1281</v>
+      </c>
+      <c r="L478" s="139"/>
+      <c r="M478" s="139"/>
+      <c r="N478" s="139"/>
+      <c r="O478" s="139"/>
+      <c r="P478" s="139"/>
+      <c r="Q478" s="139"/>
+      <c r="R478" s="139"/>
+      <c r="S478" s="139"/>
+      <c r="T478" s="139"/>
+      <c r="U478" s="139"/>
+      <c r="V478" s="139"/>
+    </row>
+    <row r="479" spans="1:25" s="187" customFormat="1" ht="17" thickBot="1">
+      <c r="A479" s="188"/>
+      <c r="B479" s="189"/>
+      <c r="C479" s="139"/>
+      <c r="D479" s="139"/>
+      <c r="E479" s="188" t="s">
+        <v>166</v>
+      </c>
+      <c r="F479" s="204">
+        <f>F478/1000</f>
+        <v>1.258</v>
+      </c>
+      <c r="G479" s="139" t="s">
+        <v>149</v>
+      </c>
+      <c r="H479" s="201">
+        <v>42191</v>
+      </c>
+      <c r="I479" s="202">
+        <v>1</v>
+      </c>
+      <c r="J479" s="206">
+        <v>580.19000000000005</v>
+      </c>
+      <c r="K479" s="203">
+        <v>1295</v>
+      </c>
+      <c r="L479" s="139"/>
+      <c r="M479" s="139"/>
+      <c r="N479" s="139"/>
+      <c r="O479" s="139"/>
+      <c r="P479" s="139"/>
+      <c r="Q479" s="139"/>
+      <c r="R479" s="139"/>
+      <c r="S479" s="139"/>
+      <c r="T479" s="139"/>
+      <c r="U479" s="139"/>
+      <c r="V479" s="139"/>
+    </row>
+    <row r="480" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A480" s="188"/>
+      <c r="B480" s="189"/>
+      <c r="C480" s="139"/>
+      <c r="D480" s="139"/>
+      <c r="E480" s="139"/>
+      <c r="F480" s="139"/>
+      <c r="G480" s="139"/>
+      <c r="H480" s="201">
+        <v>42184</v>
+      </c>
+      <c r="I480" s="202">
+        <v>1</v>
+      </c>
+      <c r="J480" s="206">
+        <v>580.19000000000005</v>
+      </c>
+      <c r="K480" s="203">
+        <v>1295</v>
+      </c>
+      <c r="L480" s="139"/>
+      <c r="M480" s="139"/>
+      <c r="N480" s="139"/>
+      <c r="O480" s="139"/>
+      <c r="P480" s="139"/>
+      <c r="Q480" s="139"/>
+      <c r="R480" s="139"/>
+      <c r="S480" s="139"/>
+      <c r="T480" s="139"/>
+      <c r="U480" s="139"/>
+      <c r="V480" s="139"/>
+    </row>
+    <row r="481" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A481" s="188"/>
+      <c r="B481" s="189"/>
+      <c r="C481" s="139"/>
+      <c r="D481" s="142" t="s">
+        <v>159</v>
+      </c>
+      <c r="E481" s="139"/>
+      <c r="F481" s="205"/>
+      <c r="G481" s="139"/>
+      <c r="H481" s="201">
+        <v>42177</v>
+      </c>
+      <c r="I481" s="202">
+        <v>1</v>
+      </c>
+      <c r="J481" s="206">
+        <v>585.15</v>
+      </c>
+      <c r="K481" s="203">
+        <v>1301</v>
+      </c>
+      <c r="L481" s="139"/>
+      <c r="M481" s="139"/>
+      <c r="N481" s="139"/>
+      <c r="O481" s="139"/>
+      <c r="P481" s="139"/>
+      <c r="Q481" s="139"/>
+      <c r="R481" s="139"/>
+      <c r="S481" s="139"/>
+      <c r="T481" s="139"/>
+      <c r="U481" s="139"/>
+      <c r="V481" s="139"/>
+    </row>
+    <row r="482" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A482" s="188"/>
+      <c r="B482" s="189"/>
+      <c r="C482" s="139"/>
+      <c r="D482" s="139" t="s">
+        <v>160</v>
+      </c>
+      <c r="E482" s="188" t="s">
+        <v>166</v>
+      </c>
+      <c r="F482" s="139">
+        <v>21</v>
+      </c>
+      <c r="G482" s="139" t="s">
+        <v>161</v>
+      </c>
+      <c r="H482" s="201">
+        <v>42170</v>
+      </c>
+      <c r="I482" s="202">
+        <v>1</v>
+      </c>
+      <c r="J482" s="206">
+        <v>587.63</v>
+      </c>
+      <c r="K482" s="203">
+        <v>1304</v>
+      </c>
+      <c r="L482" s="139"/>
+      <c r="M482" s="139"/>
+      <c r="N482" s="139"/>
+      <c r="O482" s="139"/>
+      <c r="P482" s="139"/>
+      <c r="Q482" s="139"/>
+      <c r="R482" s="139"/>
+      <c r="S482" s="139"/>
+      <c r="T482" s="139"/>
+      <c r="U482" s="139"/>
+      <c r="V482" s="139"/>
+    </row>
+    <row r="483" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A483" s="188"/>
+      <c r="B483" s="189"/>
+      <c r="C483" s="139"/>
+      <c r="D483" s="139" t="s">
+        <v>162</v>
+      </c>
+      <c r="E483" s="188" t="s">
+        <v>166</v>
+      </c>
+      <c r="F483" s="139">
+        <f>482.06/1000</f>
+        <v>0.48205999999999999</v>
+      </c>
+      <c r="G483" s="139" t="s">
+        <v>149</v>
+      </c>
+      <c r="H483" s="201">
+        <v>42163</v>
+      </c>
+      <c r="I483" s="202">
+        <v>1</v>
+      </c>
+      <c r="J483" s="206">
+        <v>587.63</v>
+      </c>
+      <c r="K483" s="203">
+        <v>1304</v>
+      </c>
+      <c r="L483" s="139"/>
+      <c r="M483" s="139"/>
+      <c r="N483" s="139"/>
+      <c r="O483" s="139"/>
+      <c r="P483" s="139"/>
+      <c r="Q483" s="139"/>
+      <c r="R483" s="139"/>
+      <c r="S483" s="139"/>
+      <c r="T483" s="139"/>
+      <c r="U483" s="139"/>
+      <c r="V483" s="139"/>
+    </row>
+    <row r="484" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A484" s="188"/>
+      <c r="B484" s="189"/>
+      <c r="C484" s="139"/>
+      <c r="D484" s="139" t="s">
+        <v>163</v>
+      </c>
+      <c r="E484" s="188" t="s">
+        <v>166</v>
+      </c>
+      <c r="F484" s="205">
+        <f>8/1000</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G484" s="139" t="s">
+        <v>149</v>
+      </c>
+      <c r="H484" s="201">
+        <v>42156</v>
+      </c>
+      <c r="I484" s="202">
+        <v>1</v>
+      </c>
+      <c r="J484" s="206">
+        <v>587.63</v>
+      </c>
+      <c r="K484" s="203">
+        <v>1304</v>
+      </c>
+      <c r="L484" s="139"/>
+      <c r="M484" s="139"/>
+      <c r="N484" s="139"/>
+      <c r="O484" s="139"/>
+      <c r="P484" s="139"/>
+      <c r="Q484" s="139"/>
+      <c r="R484" s="139"/>
+      <c r="S484" s="139"/>
+      <c r="T484" s="139"/>
+      <c r="U484" s="139"/>
+      <c r="V484" s="139"/>
+    </row>
+    <row r="485" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A485" s="188"/>
+      <c r="B485" s="189"/>
+      <c r="C485" s="139"/>
+      <c r="D485" s="139"/>
+      <c r="E485" s="139"/>
+      <c r="F485" s="139"/>
+      <c r="G485" s="139"/>
+      <c r="H485" s="201">
+        <v>42149</v>
+      </c>
+      <c r="I485" s="202">
+        <v>1</v>
+      </c>
+      <c r="J485" s="206">
+        <v>591.76</v>
+      </c>
+      <c r="K485" s="203">
+        <v>1309</v>
+      </c>
+      <c r="L485" s="139"/>
+      <c r="M485" s="139"/>
+      <c r="N485" s="139"/>
+      <c r="O485" s="139"/>
+      <c r="P485" s="139"/>
+      <c r="Q485" s="139"/>
+      <c r="R485" s="139"/>
+      <c r="S485" s="139"/>
+      <c r="T485" s="139"/>
+      <c r="U485" s="139"/>
+      <c r="V485" s="139"/>
+    </row>
+    <row r="486" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A486" s="188"/>
+      <c r="B486" s="189"/>
+      <c r="C486" s="139"/>
+      <c r="D486" s="139" t="s">
+        <v>164</v>
+      </c>
+      <c r="E486" s="188" t="s">
+        <v>166</v>
+      </c>
+      <c r="F486" s="205">
+        <f>(F484+F483+F476)*1.21</f>
+        <v>1.2580007</v>
+      </c>
+      <c r="G486" s="139" t="s">
+        <v>165</v>
+      </c>
+      <c r="H486" s="201">
+        <v>42142</v>
+      </c>
+      <c r="I486" s="202">
+        <v>1</v>
+      </c>
+      <c r="J486" s="206">
+        <v>594.24</v>
+      </c>
+      <c r="K486" s="203">
+        <v>1312</v>
+      </c>
+      <c r="L486" s="139"/>
+      <c r="M486" s="139"/>
+      <c r="N486" s="139"/>
+      <c r="O486" s="139"/>
+      <c r="P486" s="139"/>
+      <c r="Q486" s="139"/>
+      <c r="R486" s="139"/>
+      <c r="S486" s="139"/>
+      <c r="T486" s="139"/>
+      <c r="U486" s="139"/>
+      <c r="V486" s="139"/>
+    </row>
+    <row r="487" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A487" s="188"/>
+      <c r="B487" s="189"/>
+      <c r="C487" s="139"/>
+      <c r="D487" s="139"/>
+      <c r="E487" s="139"/>
+      <c r="F487" s="139"/>
+      <c r="G487" s="139"/>
+      <c r="H487" s="201">
+        <v>42135</v>
+      </c>
+      <c r="I487" s="202">
+        <v>1</v>
+      </c>
+      <c r="J487" s="206">
+        <v>595.05999999999995</v>
+      </c>
+      <c r="K487" s="203">
+        <v>1313</v>
+      </c>
+      <c r="L487" s="139"/>
+      <c r="M487" s="139"/>
+      <c r="N487" s="139"/>
+      <c r="O487" s="139"/>
+      <c r="P487" s="139"/>
+      <c r="Q487" s="139"/>
+      <c r="R487" s="139"/>
+      <c r="S487" s="139"/>
+      <c r="T487" s="139"/>
+      <c r="U487" s="139"/>
+      <c r="V487" s="139"/>
+    </row>
+    <row r="488" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A488" s="188"/>
+      <c r="B488" s="189"/>
+      <c r="C488" s="139"/>
+      <c r="D488" s="139"/>
+      <c r="E488" s="139"/>
+      <c r="F488" s="139"/>
+      <c r="G488" s="139"/>
+      <c r="H488" s="201">
+        <v>42128</v>
+      </c>
+      <c r="I488" s="202">
+        <v>1</v>
+      </c>
+      <c r="J488" s="206">
+        <v>590.11</v>
+      </c>
+      <c r="K488" s="203">
+        <v>1307</v>
+      </c>
+      <c r="L488" s="139"/>
+      <c r="M488" s="139"/>
+      <c r="N488" s="139"/>
+      <c r="O488" s="139"/>
+      <c r="P488" s="139"/>
+      <c r="Q488" s="139"/>
+      <c r="R488" s="139"/>
+      <c r="S488" s="139"/>
+      <c r="T488" s="139"/>
+      <c r="U488" s="139"/>
+      <c r="V488" s="139"/>
+    </row>
+    <row r="489" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A489" s="188"/>
+      <c r="B489" s="189"/>
+      <c r="C489" s="139"/>
+      <c r="D489" s="139"/>
+      <c r="E489" s="139"/>
+      <c r="F489" s="139"/>
+      <c r="G489" s="139"/>
+      <c r="H489" s="201">
+        <v>42121</v>
+      </c>
+      <c r="I489" s="202">
+        <v>1</v>
+      </c>
+      <c r="J489" s="206">
+        <v>591.76</v>
+      </c>
+      <c r="K489" s="203">
+        <v>1309</v>
+      </c>
+      <c r="L489" s="139"/>
+      <c r="M489" s="139"/>
+      <c r="N489" s="139"/>
+      <c r="O489" s="139"/>
+      <c r="P489" s="139"/>
+      <c r="Q489" s="139"/>
+      <c r="R489" s="139"/>
+      <c r="S489" s="139"/>
+      <c r="T489" s="139"/>
+      <c r="U489" s="139"/>
+      <c r="V489" s="139"/>
+    </row>
+    <row r="490" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A490" s="188"/>
+      <c r="B490" s="189"/>
+      <c r="C490" s="139"/>
+      <c r="D490" s="139"/>
+      <c r="E490" s="139"/>
+      <c r="F490" s="139"/>
+      <c r="G490" s="139"/>
+      <c r="H490" s="201">
+        <v>42114</v>
+      </c>
+      <c r="I490" s="202">
+        <v>1</v>
+      </c>
+      <c r="J490" s="206">
+        <v>576.88</v>
+      </c>
+      <c r="K490" s="203">
+        <v>1291</v>
+      </c>
+      <c r="L490" s="139"/>
+      <c r="M490" s="139"/>
+      <c r="N490" s="139"/>
+      <c r="O490" s="139"/>
+      <c r="P490" s="139"/>
+      <c r="Q490" s="139"/>
+      <c r="R490" s="139"/>
+      <c r="S490" s="139"/>
+      <c r="T490" s="139"/>
+      <c r="U490" s="139"/>
+      <c r="V490" s="139"/>
+    </row>
+    <row r="491" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A491" s="188"/>
+      <c r="B491" s="189"/>
+      <c r="C491" s="139"/>
+      <c r="D491" s="139"/>
+      <c r="E491" s="139"/>
+      <c r="F491" s="139"/>
+      <c r="G491" s="139"/>
+      <c r="H491" s="201">
+        <v>42107</v>
+      </c>
+      <c r="I491" s="202">
+        <v>1</v>
+      </c>
+      <c r="J491" s="206">
+        <v>553.74</v>
+      </c>
+      <c r="K491" s="203">
+        <v>1263</v>
+      </c>
+      <c r="L491" s="139"/>
+      <c r="M491" s="139"/>
+      <c r="N491" s="139"/>
+      <c r="O491" s="139"/>
+      <c r="P491" s="139"/>
+      <c r="Q491" s="139"/>
+      <c r="R491" s="139"/>
+      <c r="S491" s="139"/>
+      <c r="T491" s="139"/>
+      <c r="U491" s="139"/>
+      <c r="V491" s="139"/>
+    </row>
+    <row r="492" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A492" s="188"/>
+      <c r="B492" s="189"/>
+      <c r="C492" s="139"/>
+      <c r="D492" s="139"/>
+      <c r="E492" s="139"/>
+      <c r="F492" s="139"/>
+      <c r="G492" s="139"/>
+      <c r="H492" s="201">
+        <v>42093</v>
+      </c>
+      <c r="I492" s="202">
+        <v>1</v>
+      </c>
+      <c r="J492" s="206">
+        <v>566.14</v>
+      </c>
+      <c r="K492" s="203">
+        <v>1278</v>
+      </c>
+      <c r="L492" s="139"/>
+      <c r="M492" s="139"/>
+      <c r="N492" s="139"/>
+      <c r="O492" s="139"/>
+      <c r="P492" s="139"/>
+      <c r="Q492" s="139"/>
+      <c r="R492" s="139"/>
+      <c r="S492" s="139"/>
+      <c r="T492" s="139"/>
+      <c r="U492" s="139"/>
+      <c r="V492" s="139"/>
+    </row>
+    <row r="493" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A493" s="188"/>
+      <c r="B493" s="189"/>
+      <c r="C493" s="139"/>
+      <c r="D493" s="139"/>
+      <c r="E493" s="139"/>
+      <c r="F493" s="139"/>
+      <c r="G493" s="139"/>
+      <c r="H493" s="201">
+        <v>42086</v>
+      </c>
+      <c r="I493" s="202">
+        <v>1</v>
+      </c>
+      <c r="J493" s="206">
+        <v>567.79</v>
+      </c>
+      <c r="K493" s="203">
+        <v>1280</v>
+      </c>
+      <c r="L493" s="139"/>
+      <c r="M493" s="139"/>
+      <c r="N493" s="139"/>
+      <c r="O493" s="139"/>
+      <c r="P493" s="139"/>
+      <c r="Q493" s="139"/>
+      <c r="R493" s="139"/>
+      <c r="S493" s="139"/>
+      <c r="T493" s="139"/>
+      <c r="U493" s="139"/>
+      <c r="V493" s="139"/>
+    </row>
+    <row r="494" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A494" s="188"/>
+      <c r="B494" s="189"/>
+      <c r="C494" s="188"/>
+      <c r="D494" s="188"/>
+      <c r="E494" s="188"/>
+      <c r="F494" s="139"/>
+      <c r="G494" s="139"/>
+      <c r="H494" s="201">
+        <v>42079</v>
+      </c>
+      <c r="I494" s="202">
+        <v>1</v>
+      </c>
+      <c r="J494" s="206">
+        <v>578.54</v>
+      </c>
+      <c r="K494" s="203">
+        <v>1293</v>
+      </c>
+      <c r="L494" s="188"/>
+      <c r="M494" s="188"/>
+      <c r="N494" s="188"/>
+      <c r="O494" s="188"/>
+      <c r="P494" s="188"/>
+      <c r="Q494" s="188"/>
+      <c r="R494" s="188"/>
+      <c r="S494" s="188"/>
+      <c r="T494" s="188"/>
+      <c r="U494" s="188"/>
+      <c r="V494" s="188"/>
+    </row>
+    <row r="495" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A495" s="188"/>
+      <c r="B495" s="189"/>
+      <c r="C495" s="188"/>
+      <c r="D495" s="188"/>
+      <c r="E495" s="188"/>
+      <c r="F495" s="139"/>
+      <c r="G495" s="139"/>
+      <c r="H495" s="201">
+        <v>42072</v>
+      </c>
+      <c r="I495" s="202">
+        <v>1</v>
+      </c>
+      <c r="J495" s="206">
+        <v>579.36</v>
+      </c>
+      <c r="K495" s="203">
+        <v>1294</v>
+      </c>
+      <c r="L495" s="188"/>
+      <c r="M495" s="188"/>
+      <c r="N495" s="188"/>
+      <c r="O495" s="188"/>
+      <c r="P495" s="188"/>
+      <c r="Q495" s="188"/>
+      <c r="R495" s="188"/>
+      <c r="S495" s="188"/>
+      <c r="T495" s="188"/>
+      <c r="U495" s="188"/>
+      <c r="V495" s="188"/>
+    </row>
+    <row r="496" spans="1:22" s="187" customFormat="1" ht="16">
+      <c r="A496" s="188"/>
+      <c r="B496" s="189"/>
+      <c r="C496" s="188"/>
+      <c r="D496" s="188"/>
+      <c r="E496" s="188"/>
+      <c r="F496" s="139"/>
+      <c r="G496" s="139"/>
+      <c r="H496" s="201">
+        <v>42065</v>
+      </c>
+      <c r="I496" s="202">
+        <v>1</v>
+      </c>
+      <c r="J496" s="206">
+        <v>578.54</v>
+      </c>
+      <c r="K496" s="203">
+        <v>1293</v>
+      </c>
+      <c r="L496" s="188"/>
+      <c r="M496" s="188"/>
+      <c r="N496" s="188"/>
+      <c r="O496" s="188"/>
+      <c r="P496" s="188"/>
+      <c r="Q496" s="188"/>
+      <c r="R496" s="188"/>
+      <c r="S496" s="188"/>
+      <c r="T496" s="188"/>
+      <c r="U496" s="188"/>
+      <c r="V496" s="188"/>
+    </row>
+    <row r="497" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A497" s="188"/>
+      <c r="B497" s="189"/>
+      <c r="C497" s="188"/>
+      <c r="D497" s="188"/>
+      <c r="E497" s="188"/>
+      <c r="F497" s="139"/>
+      <c r="G497" s="139"/>
+      <c r="H497" s="201">
+        <v>42058</v>
+      </c>
+      <c r="I497" s="202">
+        <v>1</v>
+      </c>
+      <c r="J497" s="206">
+        <v>569.44000000000005</v>
+      </c>
+      <c r="K497" s="203">
+        <v>1282</v>
+      </c>
+      <c r="L497" s="188"/>
+      <c r="M497" s="188"/>
+      <c r="N497" s="188"/>
+      <c r="O497" s="188"/>
+      <c r="P497" s="188"/>
+      <c r="Q497" s="188"/>
+      <c r="R497" s="188"/>
+      <c r="S497" s="188"/>
+      <c r="T497" s="188"/>
+      <c r="U497" s="188"/>
+      <c r="V497" s="188"/>
+    </row>
+    <row r="498" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A498" s="188"/>
+      <c r="B498" s="189"/>
+      <c r="C498" s="188"/>
+      <c r="D498" s="188"/>
+      <c r="E498" s="188"/>
+      <c r="F498" s="139"/>
+      <c r="G498" s="139"/>
+      <c r="H498" s="201">
+        <v>42051</v>
+      </c>
+      <c r="I498" s="202">
+        <v>1</v>
+      </c>
+      <c r="J498" s="206">
+        <v>560.35</v>
+      </c>
+      <c r="K498" s="203">
+        <v>1271</v>
+      </c>
+      <c r="L498" s="188"/>
+      <c r="M498" s="188"/>
+      <c r="N498" s="188"/>
+      <c r="O498" s="188"/>
+      <c r="P498" s="188"/>
+      <c r="Q498" s="188"/>
+      <c r="R498" s="188"/>
+      <c r="S498" s="188"/>
+      <c r="T498" s="188"/>
+      <c r="U498" s="188"/>
+      <c r="V498" s="188"/>
+    </row>
+    <row r="499" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A499" s="188"/>
+      <c r="B499" s="189"/>
+      <c r="C499" s="188"/>
+      <c r="D499" s="188"/>
+      <c r="E499" s="188"/>
+      <c r="F499" s="139"/>
+      <c r="G499" s="139"/>
+      <c r="H499" s="201">
+        <v>42044</v>
+      </c>
+      <c r="I499" s="202">
+        <v>1</v>
+      </c>
+      <c r="J499" s="206">
+        <v>525.64</v>
+      </c>
+      <c r="K499" s="203">
+        <v>1229</v>
+      </c>
+      <c r="L499" s="188"/>
+      <c r="M499" s="188"/>
+      <c r="N499" s="188"/>
+      <c r="O499" s="188"/>
+      <c r="P499" s="188"/>
+      <c r="Q499" s="188"/>
+      <c r="R499" s="188"/>
+      <c r="S499" s="188"/>
+      <c r="T499" s="188"/>
+      <c r="U499" s="188"/>
+      <c r="V499" s="188"/>
+    </row>
+    <row r="500" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A500" s="188"/>
+      <c r="B500" s="189"/>
+      <c r="C500" s="188"/>
+      <c r="D500" s="188"/>
+      <c r="E500" s="188"/>
+      <c r="F500" s="139"/>
+      <c r="G500" s="139"/>
+      <c r="H500" s="201">
+        <v>42037</v>
+      </c>
+      <c r="I500" s="202">
+        <v>1</v>
+      </c>
+      <c r="J500" s="206">
+        <v>496.72</v>
+      </c>
+      <c r="K500" s="203">
+        <v>1194</v>
+      </c>
+      <c r="L500" s="188"/>
+      <c r="M500" s="188"/>
+      <c r="N500" s="188"/>
+      <c r="O500" s="188"/>
+      <c r="P500" s="188"/>
+      <c r="Q500" s="188"/>
+      <c r="R500" s="188"/>
+      <c r="S500" s="188"/>
+      <c r="T500" s="188"/>
+      <c r="U500" s="188"/>
+      <c r="V500" s="188"/>
+    </row>
+    <row r="501" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A501" s="188"/>
+      <c r="B501" s="189"/>
+      <c r="C501" s="188"/>
+      <c r="D501" s="188"/>
+      <c r="E501" s="188"/>
+      <c r="F501" s="139"/>
+      <c r="G501" s="139"/>
+      <c r="H501" s="201">
+        <v>42030</v>
+      </c>
+      <c r="I501" s="202">
+        <v>1</v>
+      </c>
+      <c r="J501" s="206">
+        <v>490.93</v>
+      </c>
+      <c r="K501" s="203">
+        <v>1187</v>
+      </c>
+      <c r="L501" s="188"/>
+      <c r="M501" s="188"/>
+      <c r="N501" s="188"/>
+      <c r="O501" s="188"/>
+      <c r="P501" s="188"/>
+      <c r="Q501" s="188"/>
+      <c r="R501" s="188"/>
+      <c r="S501" s="188"/>
+      <c r="T501" s="188"/>
+      <c r="U501" s="188"/>
+      <c r="V501" s="188"/>
+    </row>
+    <row r="502" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A502" s="188"/>
+      <c r="B502" s="189"/>
+      <c r="C502" s="188"/>
+      <c r="D502" s="188"/>
+      <c r="E502" s="188"/>
+      <c r="F502" s="139"/>
+      <c r="G502" s="139"/>
+      <c r="H502" s="201">
+        <v>42023</v>
+      </c>
+      <c r="I502" s="202">
+        <v>1</v>
+      </c>
+      <c r="J502" s="206">
+        <v>490.93</v>
+      </c>
+      <c r="K502" s="203">
+        <v>1187</v>
+      </c>
+      <c r="L502" s="188"/>
+      <c r="M502" s="188"/>
+      <c r="N502" s="188"/>
+      <c r="O502" s="188"/>
+      <c r="P502" s="188"/>
+      <c r="Q502" s="188"/>
+      <c r="R502" s="188"/>
+      <c r="S502" s="188"/>
+      <c r="T502" s="188"/>
+      <c r="U502" s="188"/>
+      <c r="V502" s="188"/>
+    </row>
+    <row r="503" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A503" s="188"/>
+      <c r="B503" s="189"/>
+      <c r="C503" s="188"/>
+      <c r="D503" s="188"/>
+      <c r="E503" s="188"/>
+      <c r="F503" s="139"/>
+      <c r="G503" s="139"/>
+      <c r="H503" s="201">
+        <v>42016</v>
+      </c>
+      <c r="I503" s="202">
+        <v>1</v>
+      </c>
+      <c r="J503" s="206">
+        <v>502.5</v>
+      </c>
+      <c r="K503" s="203">
+        <v>1201</v>
+      </c>
+      <c r="L503" s="188"/>
+      <c r="M503" s="188"/>
+      <c r="N503" s="188"/>
+      <c r="O503" s="188"/>
+      <c r="P503" s="188"/>
+      <c r="Q503" s="188"/>
+      <c r="R503" s="188"/>
+      <c r="S503" s="188"/>
+      <c r="T503" s="188"/>
+      <c r="U503" s="188"/>
+      <c r="V503" s="188"/>
+    </row>
+    <row r="504" spans="1:25" s="187" customFormat="1" ht="16">
+      <c r="A504" s="188"/>
+      <c r="B504" s="189"/>
+      <c r="C504" s="188"/>
+      <c r="D504" s="188"/>
+      <c r="E504" s="188"/>
+      <c r="F504" s="139"/>
+      <c r="G504" s="139"/>
+      <c r="H504" s="201">
+        <v>42009</v>
+      </c>
+      <c r="I504" s="202">
+        <v>1</v>
+      </c>
+      <c r="J504" s="206">
+        <v>508.29</v>
+      </c>
+      <c r="K504" s="203">
+        <v>1208</v>
+      </c>
+      <c r="L504" s="188"/>
+      <c r="M504" s="188"/>
+      <c r="N504" s="188"/>
+      <c r="O504" s="188"/>
+      <c r="P504" s="188"/>
+      <c r="Q504" s="188"/>
+      <c r="R504" s="188"/>
+      <c r="S504" s="188"/>
+      <c r="T504" s="188"/>
+      <c r="U504" s="188"/>
+      <c r="V504" s="188"/>
+    </row>
+    <row r="505" spans="1:25" s="187" customFormat="1">
+      <c r="B505" s="189"/>
+    </row>
+    <row r="506" spans="1:25" s="187" customFormat="1">
+      <c r="B506" s="189"/>
+    </row>
+    <row r="507" spans="1:25" s="187" customFormat="1" ht="16" thickBot="1">
+      <c r="B507" s="189"/>
+    </row>
+    <row r="508" spans="1:25" s="26" customFormat="1">
+      <c r="B508" s="129"/>
+      <c r="C508" s="129" t="s">
+        <v>25</v>
+      </c>
+      <c r="D508" s="129" t="s">
+        <v>65</v>
+      </c>
+      <c r="E508" s="129"/>
+      <c r="F508" s="129" t="s">
+        <v>32</v>
+      </c>
+      <c r="G508" s="129"/>
+      <c r="H508" s="129"/>
+      <c r="I508" s="129"/>
+      <c r="J508" s="129"/>
+      <c r="K508" s="129"/>
+      <c r="L508" s="129"/>
+      <c r="M508" s="129"/>
+      <c r="N508" s="129"/>
+      <c r="O508" s="129"/>
+      <c r="P508" s="129"/>
+      <c r="Q508" s="129"/>
+      <c r="R508" s="129"/>
+      <c r="S508" s="129"/>
+      <c r="T508" s="129"/>
+      <c r="U508" s="129"/>
+    </row>
+    <row r="509" spans="1:25" customFormat="1" ht="16">
+      <c r="B509" s="207"/>
+      <c r="C509" s="144"/>
+      <c r="D509" s="139"/>
+      <c r="E509" s="139"/>
+      <c r="F509" s="139"/>
+      <c r="G509" s="139"/>
+      <c r="H509" s="139"/>
+      <c r="I509" s="139"/>
+      <c r="J509" s="139"/>
+      <c r="K509" s="139"/>
+      <c r="L509" s="139"/>
+      <c r="M509" s="139"/>
+      <c r="N509" s="139"/>
+      <c r="O509" s="139"/>
+      <c r="P509" s="139"/>
+      <c r="Q509" s="139"/>
+      <c r="R509" s="139"/>
+      <c r="S509" s="139"/>
+      <c r="T509" s="139"/>
+      <c r="U509" s="139"/>
+      <c r="V509" s="139"/>
+      <c r="W509" s="139"/>
+      <c r="X509" s="139"/>
+      <c r="Y509" s="139"/>
+    </row>
+    <row r="510" spans="1:25" customFormat="1" ht="16">
+      <c r="B510" s="207"/>
+      <c r="C510" s="187" t="s">
+        <v>171</v>
+      </c>
+      <c r="D510" s="139"/>
+      <c r="E510" s="139"/>
+      <c r="F510" s="139"/>
+      <c r="G510" s="139"/>
+      <c r="H510" s="139"/>
+      <c r="I510" s="139"/>
+      <c r="J510" s="139"/>
+      <c r="K510" s="139"/>
+      <c r="L510" s="139"/>
+      <c r="M510" s="139"/>
+      <c r="N510" s="139"/>
+      <c r="O510" s="139"/>
+      <c r="P510" s="139"/>
+      <c r="Q510" s="139"/>
+      <c r="R510" s="139"/>
+      <c r="S510" s="139"/>
+      <c r="T510" s="139"/>
+      <c r="U510" s="139"/>
+      <c r="V510" s="139"/>
+      <c r="W510" s="139"/>
+      <c r="X510" s="139"/>
+      <c r="Y510" s="139"/>
+    </row>
+    <row r="511" spans="1:25" s="187" customFormat="1">
+      <c r="B511" s="207"/>
+    </row>
+    <row r="512" spans="1:25" s="187" customFormat="1">
+      <c r="B512" s="207"/>
+    </row>
+    <row r="513" spans="2:8" s="187" customFormat="1">
+      <c r="B513" s="207"/>
+      <c r="D513" s="187" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="514" spans="2:8" s="187" customFormat="1">
+      <c r="B514" s="207"/>
+      <c r="D514" s="187" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="515" spans="2:8" s="187" customFormat="1">
+      <c r="B515" s="207"/>
+    </row>
+    <row r="516" spans="2:8" s="187" customFormat="1">
+      <c r="B516" s="207"/>
+      <c r="F516" s="187">
+        <v>0.5</v>
+      </c>
+      <c r="G516" s="187" t="s">
+        <v>149</v>
+      </c>
+      <c r="H516" s="187" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="517" spans="2:8" s="187" customFormat="1">
+      <c r="B517" s="207"/>
+      <c r="F517" s="208">
+        <f>F479</f>
+        <v>1.258</v>
+      </c>
+      <c r="G517" s="187" t="s">
+        <v>149</v>
+      </c>
+      <c r="H517" s="187" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="518" spans="2:8" s="187" customFormat="1">
+      <c r="B518" s="207"/>
+      <c r="F518" s="208">
+        <f>F516+F517</f>
+        <v>1.758</v>
+      </c>
+      <c r="G518" s="187" t="s">
+        <v>149</v>
+      </c>
+      <c r="H518" s="187" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="519" spans="2:8" s="187" customFormat="1">
+      <c r="B519" s="207"/>
+    </row>
+    <row r="520" spans="2:8" s="187" customFormat="1">
+      <c r="B520" s="207"/>
+      <c r="F520" s="187">
+        <f>F483</f>
+        <v>0.48205999999999999</v>
+      </c>
+      <c r="G520" s="187" t="s">
+        <v>149</v>
+      </c>
+      <c r="H520" s="187" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="521" spans="2:8" s="187" customFormat="1">
+      <c r="B521" s="207"/>
+      <c r="F521" s="208">
+        <f>F484</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G521" s="187" t="s">
+        <v>149</v>
+      </c>
+      <c r="H521" s="187" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="522" spans="2:8" s="187" customFormat="1">
+      <c r="B522" s="207"/>
+      <c r="F522" s="187">
+        <f>F482</f>
+        <v>21</v>
+      </c>
+      <c r="G522" s="187" t="s">
+        <v>161</v>
+      </c>
+      <c r="H522" s="187" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="523" spans="2:8" s="187" customFormat="1">
+      <c r="B523" s="207"/>
+    </row>
+    <row r="524" spans="2:8" s="187" customFormat="1">
+      <c r="B524" s="207"/>
+    </row>
+    <row r="525" spans="2:8" s="187" customFormat="1">
+      <c r="B525" s="207"/>
+    </row>
+    <row r="526" spans="2:8" s="187" customFormat="1">
+      <c r="B526" s="207"/>
+    </row>
+    <row r="527" spans="2:8" s="187" customFormat="1">
+      <c r="B527" s="207"/>
+      <c r="F527" s="209">
+        <f>F518/1.21-F521-F520</f>
+        <v>0.96283256198347122</v>
+      </c>
+      <c r="G527" s="187" t="s">
+        <v>149</v>
+      </c>
+      <c r="H527" s="187" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="528" spans="2:8" s="187" customFormat="1">
+      <c r="B528" s="207"/>
+      <c r="F528" s="210">
+        <f>F527/F11</f>
+        <v>2.9081568260948144E-2</v>
+      </c>
+      <c r="G528" s="187" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="529" spans="2:2" s="187" customFormat="1">
+      <c r="B529" s="207"/>
+    </row>
+    <row r="530" spans="2:2" s="187" customFormat="1">
+      <c r="B530" s="207"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C281" r:id="rId1"/>
+    <hyperlink ref="C470" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Published state of ETDataset on July 23 2020
</commit_message>
<xml_diff>
--- a/carriers_source_analyses/biodiesel.carrier.xlsx
+++ b/carriers_source_analyses/biodiesel.carrier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/carriers_source_analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/carriers_source_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C27C0C-F909-BB42-A20A-0AF60439E9CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5410209C-E5BC-674D-A7C7-391DDF142F77}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="17540" tabRatio="762" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="17540" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -43,6 +43,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -51,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="186">
   <si>
     <t>Source</t>
   </si>
@@ -670,6 +676,12 @@
     <t>This sheet summarizes all carrier attributes formatted in the way they are used by the Energy Transition Model. This sheet contains only pure carrier values. For some countries and carriers Fuel Chain Emissions are defined (only for NL); if so these FCE are documented in a separate sheet (e.g. nl_fce). Use the Excel formulas to find the original data and sources for these numbers. 
 - The carrier analysis can be imported on ETSource by running the following rake task: rake import:carrier CARRIER="carrier name" (eg rake import:carrier CARRIER=crude_oil) 
 - The fce analysis can be imported on ETSource by running the following rake task: rake import:fce DATASET="dataset" CARRIER="carrier name" (eg rake import:fce DATASET=nl CARRIER=bio_ethanol)</t>
+  </si>
+  <si>
+    <t>kg_per_liter</t>
+  </si>
+  <si>
+    <t>kg/liter</t>
   </si>
 </sst>
 </file>
@@ -1933,7 +1945,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="53" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="236">
+  <cellXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2336,6 +2348,10 @@
     <xf numFmtId="0" fontId="39" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="361">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2698,7 +2714,7 @@
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="183" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="360" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="360" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -4175,10 +4191,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:J15"/>
+  <dimension ref="B1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4351,58 +4367,76 @@
     </row>
     <row r="13" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1">
       <c r="B13" s="25"/>
-      <c r="C13" s="37" t="s">
-        <v>40</v>
+      <c r="C13" s="237" t="s">
+        <v>184</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="48">
+        <v>185</v>
+      </c>
+      <c r="E13" s="47">
         <f>'Research data'!G9</f>
-        <v>0</v>
+        <v>0.89</v>
       </c>
       <c r="F13" s="37"/>
-      <c r="G13" s="210" t="s">
-        <v>181</v>
-      </c>
+      <c r="G13" s="131"/>
       <c r="H13" s="32"/>
-      <c r="I13" s="215" t="s">
-        <v>44</v>
-      </c>
+      <c r="I13" s="132"/>
       <c r="J13" s="46"/>
     </row>
     <row r="14" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1">
       <c r="B14" s="25"/>
-      <c r="C14" s="205" t="s">
-        <v>174</v>
+      <c r="C14" s="37" t="s">
+        <v>40</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="214">
+      <c r="E14" s="48">
         <f>'Research data'!G10</f>
-        <v>7.0800000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="F14" s="37"/>
       <c r="G14" s="210" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H14" s="32"/>
       <c r="I14" s="215" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="46"/>
+    </row>
+    <row r="15" spans="2:10" s="45" customFormat="1" ht="20" thickBot="1">
+      <c r="B15" s="25"/>
+      <c r="C15" s="205" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="214">
+        <f>'Research data'!G11</f>
+        <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="F15" s="37"/>
+      <c r="G15" s="210" t="s">
+        <v>182</v>
+      </c>
+      <c r="H15" s="32"/>
+      <c r="I15" s="215" t="s">
         <v>175</v>
       </c>
-      <c r="J14" s="46"/>
-    </row>
-    <row r="15" spans="2:10" ht="20" customHeight="1" thickBot="1">
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="44"/>
+      <c r="J15" s="46"/>
+    </row>
+    <row r="16" spans="2:10" ht="20" customHeight="1" thickBot="1">
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4550,7 +4584,7 @@
         <v>51</v>
       </c>
       <c r="E11" s="124">
-        <f>'Research data'!G14</f>
+        <f>'Research data'!G15</f>
         <v>0</v>
       </c>
       <c r="F11" s="37"/>
@@ -4572,7 +4606,7 @@
         <v>51</v>
       </c>
       <c r="E12" s="124">
-        <f>'Research data'!G15</f>
+        <f>'Research data'!G16</f>
         <v>0</v>
       </c>
       <c r="F12" s="37"/>
@@ -4594,7 +4628,7 @@
         <v>51</v>
       </c>
       <c r="E13" s="124">
-        <f>'Research data'!G16</f>
+        <f>'Research data'!G17</f>
         <v>2.01E-2</v>
       </c>
       <c r="F13" s="37"/>
@@ -4616,7 +4650,7 @@
         <v>51</v>
       </c>
       <c r="E14" s="124">
-        <f>'Research data'!G17</f>
+        <f>'Research data'!G18</f>
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="F14" s="37"/>
@@ -4638,7 +4672,7 @@
         <v>51</v>
       </c>
       <c r="E15" s="124">
-        <f>'Research data'!G18</f>
+        <f>'Research data'!G19</f>
         <v>0</v>
       </c>
       <c r="F15" s="37"/>
@@ -4660,7 +4694,7 @@
         <v>51</v>
       </c>
       <c r="E16" s="124">
-        <f>'Research data'!G19</f>
+        <f>'Research data'!G20</f>
         <v>0</v>
       </c>
       <c r="F16" s="37"/>
@@ -4682,7 +4716,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="48">
-        <f>'Research data'!G20</f>
+        <f>'Research data'!G21</f>
         <v>0.2</v>
       </c>
       <c r="F17" s="37"/>
@@ -4728,7 +4762,7 @@
         <v>51</v>
       </c>
       <c r="E20" s="124">
-        <f>'Research data'!G23</f>
+        <f>'Research data'!G24</f>
         <v>0</v>
       </c>
       <c r="F20" s="37"/>
@@ -4750,7 +4784,7 @@
         <v>51</v>
       </c>
       <c r="E21" s="124">
-        <f>'Research data'!G24</f>
+        <f>'Research data'!G25</f>
         <v>1.47E-2</v>
       </c>
       <c r="F21" s="37"/>
@@ -4772,7 +4806,7 @@
         <v>51</v>
       </c>
       <c r="E22" s="124">
-        <f>'Research data'!G25</f>
+        <f>'Research data'!G26</f>
         <v>9.4000000000000004E-3</v>
       </c>
       <c r="F22" s="37"/>
@@ -4794,7 +4828,7 @@
         <v>51</v>
       </c>
       <c r="E23" s="124">
-        <f>'Research data'!G26</f>
+        <f>'Research data'!G27</f>
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="F23" s="37"/>
@@ -4816,7 +4850,7 @@
         <v>51</v>
       </c>
       <c r="E24" s="124">
-        <f>'Research data'!G27</f>
+        <f>'Research data'!G28</f>
         <v>0</v>
       </c>
       <c r="F24" s="37"/>
@@ -4838,7 +4872,7 @@
         <v>51</v>
       </c>
       <c r="E25" s="124">
-        <f>'Research data'!G28</f>
+        <f>'Research data'!G29</f>
         <v>0</v>
       </c>
       <c r="F25" s="37"/>
@@ -4860,7 +4894,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="48">
-        <f>'Research data'!G29</f>
+        <f>'Research data'!G30</f>
         <v>0.8</v>
       </c>
       <c r="F26" s="37"/>
@@ -4898,10 +4932,10 @@
   <sheetPr codeName="Sheet3">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:R36"/>
+  <dimension ref="B1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5120,23 +5154,23 @@
     </row>
     <row r="9" spans="2:18" s="6" customFormat="1" ht="17" thickBot="1">
       <c r="B9" s="5"/>
-      <c r="C9" s="137" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="137" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="137" t="s">
-        <v>40</v>
-      </c>
+      <c r="C9" s="236" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="136"/>
+      <c r="E9" s="136"/>
       <c r="F9" s="24" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="G9" s="47">
-        <v>0</v>
+        <f>I9</f>
+        <v>0.89</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="18"/>
+      <c r="I9" s="47">
+        <f>Notes!F10</f>
+        <v>0.89</v>
+      </c>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
@@ -5149,17 +5183,20 @@
     </row>
     <row r="10" spans="2:18" s="6" customFormat="1" ht="17" thickBot="1">
       <c r="B10" s="5"/>
-      <c r="C10" s="206" t="s">
-        <v>174</v>
-      </c>
-      <c r="D10" s="137"/>
-      <c r="E10" s="137"/>
+      <c r="C10" s="137" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="137" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="137" t="s">
+        <v>40</v>
+      </c>
       <c r="F10" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="214">
-        <f>P10</f>
-        <v>7.0800000000000002E-2</v>
+      <c r="G10" s="47">
+        <v>0</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="18"/>
@@ -5169,21 +5206,25 @@
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
       <c r="O10" s="16"/>
-      <c r="P10" s="214">
-        <f>Notes!G600</f>
-        <v>7.0800000000000002E-2</v>
-      </c>
+      <c r="P10" s="16"/>
       <c r="Q10" s="16"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="2:18">
-      <c r="B11" s="78"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
+    <row r="11" spans="2:18" s="6" customFormat="1" ht="17" thickBot="1">
+      <c r="B11" s="5"/>
+      <c r="C11" s="206" t="s">
+        <v>174</v>
+      </c>
+      <c r="D11" s="137"/>
+      <c r="E11" s="137"/>
+      <c r="F11" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="214">
+        <f>P11</f>
+        <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="H11" s="4"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
@@ -5191,20 +5232,21 @@
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
       <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
+      <c r="P11" s="214">
+        <f>Notes!G600</f>
+        <v>7.0800000000000002E-2</v>
+      </c>
       <c r="Q11" s="16"/>
-      <c r="R11" s="145"/>
+      <c r="R11" s="3"/>
     </row>
     <row r="12" spans="2:18">
       <c r="B12" s="78"/>
-      <c r="C12" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="83"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="114"/>
-      <c r="H12" s="84"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
       <c r="I12" s="18"/>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
@@ -5216,16 +5258,16 @@
       <c r="Q12" s="16"/>
       <c r="R12" s="145"/>
     </row>
-    <row r="13" spans="2:18" ht="17" thickBot="1">
+    <row r="13" spans="2:18">
       <c r="B13" s="78"/>
-      <c r="C13" s="136" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="131"/>
+      <c r="C13" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="114"/>
       <c r="G13" s="114"/>
-      <c r="H13" s="85"/>
+      <c r="H13" s="84"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
@@ -5235,37 +5277,27 @@
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
       <c r="Q13" s="16"/>
-      <c r="R13" s="145" t="s">
-        <v>54</v>
-      </c>
+      <c r="R13" s="145"/>
     </row>
     <row r="14" spans="2:18" ht="17" thickBot="1">
       <c r="B14" s="78"/>
-      <c r="C14" s="138" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="124">
-        <f>M14</f>
-        <v>0</v>
-      </c>
+      <c r="C14" s="136" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="131"/>
+      <c r="G14" s="114"/>
       <c r="H14" s="85"/>
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
-      <c r="M14" s="124">
-        <f>Notes!H329</f>
-        <v>0</v>
-      </c>
+      <c r="M14" s="18"/>
       <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="82"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
       <c r="R14" s="145" t="s">
         <v>54</v>
       </c>
@@ -5273,30 +5305,30 @@
     <row r="15" spans="2:18" ht="17" thickBot="1">
       <c r="B15" s="78"/>
       <c r="C15" s="138" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
+        <v>45</v>
+      </c>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
       <c r="F15" s="24" t="s">
         <v>51</v>
       </c>
       <c r="G15" s="124">
-        <f t="shared" ref="G15:G19" si="0">M15</f>
+        <f>M15</f>
         <v>0</v>
       </c>
-      <c r="H15" s="18"/>
+      <c r="H15" s="85"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
       <c r="M15" s="124">
-        <f>Notes!H330</f>
+        <f>Notes!H329</f>
         <v>0</v>
       </c>
       <c r="N15" s="18"/>
       <c r="O15" s="18"/>
       <c r="P15" s="18"/>
-      <c r="Q15" s="6"/>
+      <c r="Q15" s="82"/>
       <c r="R15" s="145" t="s">
         <v>54</v>
       </c>
@@ -5304,16 +5336,16 @@
     <row r="16" spans="2:18" ht="17" thickBot="1">
       <c r="B16" s="78"/>
       <c r="C16" s="138" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+        <v>46</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
       <c r="F16" s="24" t="s">
         <v>51</v>
       </c>
       <c r="G16" s="124">
-        <f t="shared" si="0"/>
-        <v>2.01E-2</v>
+        <f t="shared" ref="G16:G20" si="0">M16</f>
+        <v>0</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
@@ -5321,8 +5353,8 @@
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
       <c r="M16" s="124">
-        <f>Notes!H331</f>
-        <v>2.01E-2</v>
+        <f>Notes!H330</f>
+        <v>0</v>
       </c>
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
@@ -5335,7 +5367,7 @@
     <row r="17" spans="2:18" ht="17" thickBot="1">
       <c r="B17" s="78"/>
       <c r="C17" s="138" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
@@ -5344,7 +5376,7 @@
       </c>
       <c r="G17" s="124">
         <f t="shared" si="0"/>
-        <v>5.9999999999999995E-4</v>
+        <v>2.01E-2</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
@@ -5352,8 +5384,8 @@
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
       <c r="M17" s="124">
-        <f>Notes!H332</f>
-        <v>5.9999999999999995E-4</v>
+        <f>Notes!H331</f>
+        <v>2.01E-2</v>
       </c>
       <c r="N17" s="18"/>
       <c r="O17" s="18"/>
@@ -5366,30 +5398,30 @@
     <row r="18" spans="2:18" ht="17" thickBot="1">
       <c r="B18" s="78"/>
       <c r="C18" s="138" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="89"/>
-      <c r="E18" s="89"/>
+        <v>49</v>
+      </c>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="24" t="s">
         <v>51</v>
       </c>
       <c r="G18" s="124">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="85"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H18" s="18"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
       <c r="M18" s="124">
-        <f>Notes!H333</f>
-        <v>0</v>
+        <f>Notes!H332</f>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="N18" s="18"/>
       <c r="O18" s="18"/>
       <c r="P18" s="18"/>
-      <c r="Q18" s="82"/>
+      <c r="Q18" s="6"/>
       <c r="R18" s="145" t="s">
         <v>54</v>
       </c>
@@ -5397,10 +5429,10 @@
     <row r="19" spans="2:18" ht="17" thickBot="1">
       <c r="B19" s="78"/>
       <c r="C19" s="138" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
+        <v>40</v>
+      </c>
+      <c r="D19" s="89"/>
+      <c r="E19" s="89"/>
       <c r="F19" s="24" t="s">
         <v>51</v>
       </c>
@@ -5408,13 +5440,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H19" s="18"/>
+      <c r="H19" s="85"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
       <c r="M19" s="124">
-        <f>Notes!H334</f>
+        <f>Notes!H333</f>
         <v>0</v>
       </c>
       <c r="N19" s="18"/>
@@ -5428,59 +5460,69 @@
     <row r="20" spans="2:18" ht="17" thickBot="1">
       <c r="B20" s="78"/>
       <c r="C20" s="138" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
       <c r="F20" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="48">
-        <f>M20</f>
-        <v>0.2</v>
+        <v>51</v>
+      </c>
+      <c r="G20" s="124">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18"/>
       <c r="L20" s="18"/>
-      <c r="M20" s="48">
-        <v>0.2</v>
+      <c r="M20" s="124">
+        <f>Notes!H334</f>
+        <v>0</v>
       </c>
       <c r="N20" s="18"/>
       <c r="O20" s="18"/>
       <c r="P20" s="18"/>
       <c r="Q20" s="82"/>
       <c r="R20" s="145" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="17" thickBot="1">
       <c r="B21" s="78"/>
-      <c r="C21" s="136"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="131"/>
-      <c r="G21" s="131"/>
-      <c r="H21" s="85"/>
+      <c r="C21" s="138" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="48">
+        <f>M21</f>
+        <v>0.2</v>
+      </c>
+      <c r="H21" s="18"/>
       <c r="I21" s="18"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18"/>
       <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
+      <c r="M21" s="48">
+        <v>0.2</v>
+      </c>
       <c r="N21" s="18"/>
       <c r="O21" s="18"/>
       <c r="P21" s="18"/>
       <c r="Q21" s="82"/>
-      <c r="R21" s="145"/>
+      <c r="R21" s="145" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="22" spans="2:18" ht="17" thickBot="1">
       <c r="B22" s="78"/>
-      <c r="C22" s="136" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" s="90"/>
-      <c r="E22" s="90"/>
+      <c r="C22" s="136"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="91"/>
       <c r="F22" s="131"/>
       <c r="G22" s="131"/>
       <c r="H22" s="85"/>
@@ -5488,38 +5530,28 @@
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
-      <c r="M22" s="131"/>
+      <c r="M22" s="18"/>
       <c r="N22" s="18"/>
       <c r="O22" s="18"/>
       <c r="P22" s="18"/>
-      <c r="Q22" s="80"/>
-      <c r="R22" s="145" t="s">
-        <v>54</v>
-      </c>
+      <c r="Q22" s="82"/>
+      <c r="R22" s="145"/>
     </row>
     <row r="23" spans="2:18" ht="17" thickBot="1">
       <c r="B23" s="78"/>
-      <c r="C23" s="138" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="93"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="G23" s="48">
-        <f>M23</f>
-        <v>0</v>
-      </c>
+      <c r="C23" s="136" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="131"/>
+      <c r="G23" s="131"/>
       <c r="H23" s="85"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="18"/>
-      <c r="M23" s="48">
-        <f>Notes!H346</f>
-        <v>0</v>
-      </c>
+      <c r="M23" s="131"/>
       <c r="N23" s="18"/>
       <c r="O23" s="18"/>
       <c r="P23" s="18"/>
@@ -5531,27 +5563,30 @@
     <row r="24" spans="2:18" ht="17" thickBot="1">
       <c r="B24" s="78"/>
       <c r="C24" s="138" t="s">
-        <v>46</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
       <c r="F24" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="G24" s="124">
-        <f t="shared" ref="G24:G29" si="1">M24</f>
-        <v>1.47E-2</v>
-      </c>
+      <c r="G24" s="48">
+        <f>M24</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="85"/>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
-      <c r="M24" s="124">
-        <f>Notes!H347</f>
-        <v>1.47E-2</v>
+      <c r="M24" s="48">
+        <f>Notes!H346</f>
+        <v>0</v>
       </c>
       <c r="N24" s="18"/>
       <c r="O24" s="18"/>
       <c r="P24" s="18"/>
-      <c r="Q24" s="82"/>
+      <c r="Q24" s="80"/>
       <c r="R24" s="145" t="s">
         <v>54</v>
       </c>
@@ -5559,22 +5594,22 @@
     <row r="25" spans="2:18" ht="17" thickBot="1">
       <c r="B25" s="78"/>
       <c r="C25" s="138" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F25" s="24" t="s">
         <v>51</v>
       </c>
       <c r="G25" s="124">
-        <f t="shared" si="1"/>
-        <v>9.4000000000000004E-3</v>
+        <f t="shared" ref="G25:G30" si="1">M25</f>
+        <v>1.47E-2</v>
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18"/>
       <c r="L25" s="18"/>
       <c r="M25" s="124">
-        <f>Notes!H348</f>
-        <v>9.4000000000000004E-3</v>
+        <f>Notes!H347</f>
+        <v>1.47E-2</v>
       </c>
       <c r="N25" s="18"/>
       <c r="O25" s="18"/>
@@ -5587,22 +5622,22 @@
     <row r="26" spans="2:18" ht="17" thickBot="1">
       <c r="B26" s="78"/>
       <c r="C26" s="138" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F26" s="24" t="s">
         <v>51</v>
       </c>
       <c r="G26" s="124">
         <f t="shared" si="1"/>
-        <v>6.9999999999999999E-4</v>
+        <v>9.4000000000000004E-3</v>
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
       <c r="M26" s="124">
-        <f>Notes!H349</f>
-        <v>6.9999999999999999E-4</v>
+        <f>Notes!H348</f>
+        <v>9.4000000000000004E-3</v>
       </c>
       <c r="N26" s="18"/>
       <c r="O26" s="18"/>
@@ -5615,22 +5650,22 @@
     <row r="27" spans="2:18" ht="17" thickBot="1">
       <c r="B27" s="78"/>
       <c r="C27" s="138" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>51</v>
       </c>
       <c r="G27" s="124">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
       <c r="L27" s="18"/>
       <c r="M27" s="124">
-        <f>Notes!H350</f>
-        <v>0</v>
+        <f>Notes!H349</f>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="N27" s="18"/>
       <c r="O27" s="18"/>
@@ -5643,7 +5678,7 @@
     <row r="28" spans="2:18" ht="17" thickBot="1">
       <c r="B28" s="78"/>
       <c r="C28" s="138" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F28" s="24" t="s">
         <v>51</v>
@@ -5657,13 +5692,13 @@
       <c r="K28" s="18"/>
       <c r="L28" s="18"/>
       <c r="M28" s="124">
-        <f>Notes!H351</f>
+        <f>Notes!H350</f>
         <v>0</v>
       </c>
       <c r="N28" s="18"/>
       <c r="O28" s="18"/>
       <c r="P28" s="18"/>
-      <c r="Q28" s="85"/>
+      <c r="Q28" s="82"/>
       <c r="R28" s="145" t="s">
         <v>54</v>
       </c>
@@ -5671,52 +5706,76 @@
     <row r="29" spans="2:18" ht="17" thickBot="1">
       <c r="B29" s="78"/>
       <c r="C29" s="138" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="48">
+        <v>51</v>
+      </c>
+      <c r="G29" s="124">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
-      <c r="M29" s="48">
-        <v>0.8</v>
+      <c r="M29" s="124">
+        <f>Notes!H351</f>
+        <v>0</v>
       </c>
       <c r="N29" s="18"/>
       <c r="O29" s="18"/>
       <c r="P29" s="18"/>
       <c r="Q29" s="85"/>
       <c r="R29" s="145" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" ht="17" thickBot="1">
+      <c r="B30" s="78"/>
+      <c r="C30" s="138" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" s="48">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="48">
+        <v>0.8</v>
+      </c>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="85"/>
+      <c r="R30" s="145" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="2:18" ht="17" thickBot="1">
-      <c r="B30" s="92"/>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="94"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="94"/>
-      <c r="I30" s="94"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="94"/>
-      <c r="M30" s="94"/>
-      <c r="N30" s="94"/>
-      <c r="O30" s="94"/>
-      <c r="P30" s="94"/>
-      <c r="Q30" s="94"/>
-      <c r="R30" s="95"/>
-    </row>
-    <row r="31" spans="2:18">
-      <c r="O31" s="18"/>
-      <c r="P31" s="18"/>
+    <row r="31" spans="2:18" ht="17" thickBot="1">
+      <c r="B31" s="92"/>
+      <c r="C31" s="94"/>
+      <c r="D31" s="94"/>
+      <c r="E31" s="94"/>
+      <c r="F31" s="94"/>
+      <c r="G31" s="94"/>
+      <c r="H31" s="94"/>
+      <c r="I31" s="94"/>
+      <c r="J31" s="94"/>
+      <c r="K31" s="94"/>
+      <c r="L31" s="94"/>
+      <c r="M31" s="94"/>
+      <c r="N31" s="94"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="94"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="95"/>
     </row>
     <row r="32" spans="2:18">
       <c r="O32" s="18"/>
@@ -5735,7 +5794,11 @@
       <c r="P35" s="18"/>
     </row>
     <row r="36" spans="15:18">
-      <c r="R36" s="145"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+    </row>
+    <row r="37" spans="15:18">
+      <c r="R37" s="145"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6103,7 +6166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AI631"/>
   <sheetViews>
-    <sheetView topLeftCell="A570" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F528" sqref="F528"/>
     </sheetView>
   </sheetViews>

</xml_diff>